<commit_message>
Added mse_vec-output from getPerceptronWeights for plotting of MSE
</commit_message>
<xml_diff>
--- a/Handwritten numbers/tables/confusion_matrix_template_for_handwritten_numbers.xlsx
+++ b/Handwritten numbers/tables/confusion_matrix_template_for_handwritten_numbers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\OneDrive\Dokumenter\3.klasse\Estimering\Classification_project\MNist_ttt4275\MNist_ttt4275\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\OneDrive\Dokumenter\3.klasse\Estimering\TTT4275-Project\Handwritten numbers\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECF8ED9-24DC-4908-8395-E323A427E479}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47900AB7-4A0E-4907-9BE5-014D4E7F3B6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{93388D62-B026-4318-80F4-EFF80010564F}"/>
   </bookViews>
@@ -574,7 +574,208 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="39">
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF00B050"/>
@@ -987,7 +1188,7 @@
   <dimension ref="B1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1046,31 +1247,31 @@
         <v>0</v>
       </c>
       <c r="C3" s="4">
-        <v>973</v>
+        <v>955</v>
       </c>
       <c r="D3" s="5">
         <v>1</v>
       </c>
       <c r="E3" s="5">
+        <v>3</v>
+      </c>
+      <c r="F3" s="5">
         <v>1</v>
       </c>
-      <c r="F3" s="5">
-        <v>0</v>
-      </c>
       <c r="G3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I3" s="5">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="J3" s="5">
         <v>1</v>
       </c>
       <c r="K3" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L3" s="6">
         <v>0</v>
@@ -1078,11 +1279,11 @@
       <c r="M3" s="30"/>
       <c r="N3" s="19">
         <f>SUM(D3:L3)/SUM(C3:L3)</f>
-        <v>7.1428571428571426E-3</v>
+        <v>2.5510204081632654E-2</v>
       </c>
       <c r="O3" s="24">
         <f>100%-N3</f>
-        <v>0.99285714285714288</v>
+        <v>0.97448979591836737</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.35">
@@ -1096,25 +1297,25 @@
         <v>1129</v>
       </c>
       <c r="E4" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="8">
+        <v>0</v>
+      </c>
+      <c r="H4" s="8">
+        <v>0</v>
+      </c>
+      <c r="I4" s="8">
+        <v>2</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0</v>
+      </c>
+      <c r="K4" s="8">
         <v>1</v>
-      </c>
-      <c r="H4" s="8">
-        <v>1</v>
-      </c>
-      <c r="I4" s="8">
-        <v>1</v>
-      </c>
-      <c r="J4" s="8">
-        <v>0</v>
-      </c>
-      <c r="K4" s="8">
-        <v>0</v>
       </c>
       <c r="L4" s="9">
         <v>0</v>
@@ -1134,31 +1335,31 @@
         <v>5</v>
       </c>
       <c r="C5" s="7">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D5" s="8">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E5" s="8">
-        <v>992</v>
+        <v>947</v>
       </c>
       <c r="F5" s="8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G5" s="8">
+        <v>4</v>
+      </c>
+      <c r="H5" s="8">
         <v>1</v>
       </c>
-      <c r="H5" s="8">
-        <v>0</v>
-      </c>
       <c r="I5" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J5" s="8">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="K5" s="8">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="L5" s="9">
         <v>0</v>
@@ -1166,11 +1367,11 @@
       <c r="M5" s="30"/>
       <c r="N5" s="20">
         <f>SUM(C5,D5,F5:L5)/SUM(C5:L5)</f>
-        <v>3.875968992248062E-2</v>
+        <v>8.2364341085271311E-2</v>
       </c>
       <c r="O5" s="25">
         <f t="shared" si="0"/>
-        <v>0.96124031007751942</v>
+        <v>0.91763565891472865</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.35">
@@ -1181,40 +1382,40 @@
         <v>0</v>
       </c>
       <c r="D6" s="8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E6" s="8">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F6" s="8">
-        <v>970</v>
+        <v>946</v>
       </c>
       <c r="G6" s="8">
         <v>1</v>
       </c>
       <c r="H6" s="8">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I6" s="8">
         <v>0</v>
       </c>
       <c r="J6" s="8">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="K6" s="8">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="L6" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M6" s="30"/>
       <c r="N6" s="20">
         <f>SUM(C6:E6,G6:L6)/SUM(C6:L6)</f>
-        <v>3.9603960396039604E-2</v>
+        <v>6.3366336633663367E-2</v>
       </c>
       <c r="O6" s="25">
         <f t="shared" si="0"/>
-        <v>0.96039603960396036</v>
+        <v>0.93663366336633658</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.35">
@@ -1225,40 +1426,40 @@
         <v>0</v>
       </c>
       <c r="D7" s="8">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E7" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F7" s="8">
         <v>0</v>
       </c>
       <c r="G7" s="8">
-        <v>944</v>
+        <v>900</v>
       </c>
       <c r="H7" s="8">
         <v>0</v>
       </c>
       <c r="I7" s="8">
+        <v>12</v>
+      </c>
+      <c r="J7" s="8">
+        <v>2</v>
+      </c>
+      <c r="K7" s="8">
         <v>3</v>
       </c>
-      <c r="J7" s="8">
-        <v>5</v>
-      </c>
-      <c r="K7" s="8">
-        <v>1</v>
-      </c>
       <c r="L7" s="9">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="M7" s="30"/>
       <c r="N7" s="20">
         <f>SUM(C7:F7,H7:L7)/SUM(C7:L7)</f>
-        <v>3.8696537678207736E-2</v>
+        <v>8.3503054989816694E-2</v>
       </c>
       <c r="O7" s="25">
         <f t="shared" si="0"/>
-        <v>0.96130346232179231</v>
+        <v>0.91649694501018331</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.35">
@@ -1266,31 +1467,31 @@
         <v>6</v>
       </c>
       <c r="C8" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D8" s="8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E8" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F8" s="8">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="G8" s="8">
+        <v>7</v>
+      </c>
+      <c r="H8" s="8">
+        <v>828</v>
+      </c>
+      <c r="I8" s="8">
+        <v>7</v>
+      </c>
+      <c r="J8" s="8">
         <v>2</v>
       </c>
-      <c r="H8" s="8">
-        <v>860</v>
-      </c>
-      <c r="I8" s="8">
-        <v>5</v>
-      </c>
-      <c r="J8" s="8">
-        <v>1</v>
-      </c>
       <c r="K8" s="8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L8" s="9">
         <v>4</v>
@@ -1298,11 +1499,11 @@
       <c r="M8" s="30"/>
       <c r="N8" s="20">
         <f>SUM(C8:G8,I8:L8)/SUM(C8:L8)</f>
-        <v>3.5874439461883408E-2</v>
+        <v>7.1748878923766815E-2</v>
       </c>
       <c r="O8" s="25">
         <f t="shared" si="0"/>
-        <v>0.9641255605381166</v>
+        <v>0.9282511210762332</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.35">
@@ -1310,31 +1511,31 @@
         <v>7</v>
       </c>
       <c r="C9" s="7">
+        <v>8</v>
+      </c>
+      <c r="D9" s="8">
         <v>4</v>
       </c>
-      <c r="D9" s="8">
-        <v>2</v>
-      </c>
       <c r="E9" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F9" s="8">
         <v>0</v>
       </c>
       <c r="G9" s="8">
+        <v>11</v>
+      </c>
+      <c r="H9" s="8">
+        <v>10</v>
+      </c>
+      <c r="I9" s="8">
+        <v>918</v>
+      </c>
+      <c r="J9" s="8">
+        <v>0</v>
+      </c>
+      <c r="K9" s="8">
         <v>3</v>
-      </c>
-      <c r="H9" s="8">
-        <v>5</v>
-      </c>
-      <c r="I9" s="8">
-        <v>944</v>
-      </c>
-      <c r="J9" s="8">
-        <v>0</v>
-      </c>
-      <c r="K9" s="8">
-        <v>0</v>
       </c>
       <c r="L9" s="9">
         <v>0</v>
@@ -1342,11 +1543,11 @@
       <c r="M9" s="30"/>
       <c r="N9" s="20">
         <f>SUM(C9:H9,J9:L9)/SUM(C9:L9)</f>
-        <v>1.4613778705636743E-2</v>
+        <v>4.1753653444676408E-2</v>
       </c>
       <c r="O9" s="25">
         <f t="shared" si="0"/>
-        <v>0.98538622129436326</v>
+        <v>0.95824634655532359</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.35">
@@ -1357,17 +1558,17 @@
         <v>0</v>
       </c>
       <c r="D10" s="8">
+        <v>38</v>
+      </c>
+      <c r="E10" s="8">
+        <v>13</v>
+      </c>
+      <c r="F10" s="8">
+        <v>1</v>
+      </c>
+      <c r="G10" s="8">
         <v>14</v>
       </c>
-      <c r="E10" s="8">
-        <v>6</v>
-      </c>
-      <c r="F10" s="8">
-        <v>2</v>
-      </c>
-      <c r="G10" s="8">
-        <v>4</v>
-      </c>
       <c r="H10" s="8">
         <v>0</v>
       </c>
@@ -1375,22 +1576,22 @@
         <v>0</v>
       </c>
       <c r="J10" s="8">
-        <v>992</v>
+        <v>925</v>
       </c>
       <c r="K10" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L10" s="9">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="M10" s="30"/>
       <c r="N10" s="20">
         <f>SUM(C10:I10,K10:L10)/SUM(C10:L10)</f>
-        <v>3.5019455252918288E-2</v>
+        <v>0.10019455252918288</v>
       </c>
       <c r="O10" s="25">
         <f t="shared" si="0"/>
-        <v>0.96498054474708173</v>
+        <v>0.89980544747081714</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.35">
@@ -1398,31 +1599,31 @@
         <v>2</v>
       </c>
       <c r="C11" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F11" s="8">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="G11" s="8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H11" s="8">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="I11" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J11" s="8">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="K11" s="8">
-        <v>920</v>
+        <v>885</v>
       </c>
       <c r="L11" s="9">
         <v>5</v>
@@ -1430,11 +1631,11 @@
       <c r="M11" s="30"/>
       <c r="N11" s="20">
         <f>SUM(C11:J11,L11)/SUM(C11:L11)</f>
-        <v>5.5441478439425054E-2</v>
+        <v>9.1375770020533875E-2</v>
       </c>
       <c r="O11" s="25">
         <f t="shared" si="0"/>
-        <v>0.94455852156057496</v>
+        <v>0.90862422997946612</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1442,19 +1643,19 @@
         <v>9</v>
       </c>
       <c r="C12" s="10">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D12" s="11">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E12" s="11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F12" s="11">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G12" s="11">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="H12" s="11">
         <v>5</v>
@@ -1463,22 +1664,22 @@
         <v>1</v>
       </c>
       <c r="J12" s="11">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="K12" s="11">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="L12" s="12">
-        <v>967</v>
+        <v>913</v>
       </c>
       <c r="M12" s="30"/>
       <c r="N12" s="21">
         <f>SUM(C12:K12)/SUM(C12:L12)</f>
-        <v>4.1625371655104063E-2</v>
+        <v>9.5143706640237857E-2</v>
       </c>
       <c r="O12" s="26">
         <f t="shared" si="0"/>
-        <v>0.95837462834489595</v>
+        <v>0.90485629335976214</v>
       </c>
     </row>
     <row r="13" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1496,11 +1697,11 @@
       <c r="M13" s="31"/>
       <c r="N13" s="22">
         <f>100%-SUM(C3,D4,E5,F6,G7,H8,I9,J10,K11,L12)/SUM(C3:L12)</f>
-        <v>3.0900000000000039E-2</v>
+        <v>6.5400000000000014E-2</v>
       </c>
       <c r="O13" s="27">
         <f t="shared" si="0"/>
-        <v>0.96909999999999996</v>
+        <v>0.93459999999999999</v>
       </c>
     </row>
     <row r="14" spans="2:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
@@ -1548,50 +1749,58 @@
     <mergeCell ref="N14:O14"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:L12">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="9" operator="lessThan">
       <formula>500</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="12" operator="lessThan">
       <formula>100</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="24" priority="13" operator="between">
       <formula>50</formula>
       <formula>100</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="14" operator="greaterThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N13">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="10" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="11" operator="greaterThan">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:L16">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="7" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="8" operator="greaterThan">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O13">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="greaterThan">
       <formula>0.9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O13">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="greaterThan">
       <formula>0.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O3:O12">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+      <formula>80</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>